<commit_message>
se termina script de EmisionMotorCuentaAnonima, se creó un testRun: EmisionMotorCtaAnonima
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor_Answer_CtaAnonima.xlsx
+++ b/Sura/DataSource - Emision Motor_Answer_CtaAnonima.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Sura\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455180FD-DBF6-4CD3-A541-865A159173E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679D49FD-25F7-4CF0-B668-16B4D7A10D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="80">
   <si>
     <t>Usuario</t>
   </si>
@@ -254,26 +254,35 @@
     <t>DNICtaAnonima</t>
   </si>
   <si>
-    <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
-  </si>
-  <si>
-    <t>i-preproducciongestion.segurossura.com.ar</t>
-  </si>
-  <si>
     <t>Cuenta</t>
   </si>
   <si>
     <t>Anonima</t>
   </si>
   <si>
-    <t>prueba campaña</t>
+    <t>NroDocumento</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>su</t>
+  </si>
+  <si>
+    <t>gw</t>
+  </si>
+  <si>
+    <t>COTIZADORWEB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -312,6 +321,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333A3F"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -357,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -374,6 +389,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -415,12 +431,6 @@
         <row r="2">
           <cell r="A2" t="str">
             <v>STA017</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>ABC12STA017</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>ZAZ123STA017</v>
           </cell>
         </row>
         <row r="3">
@@ -790,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD12"/>
+  <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,9 +830,10 @@
     <col min="28" max="28" width="13.28515625" customWidth="1"/>
     <col min="29" max="29" width="13.7109375" customWidth="1"/>
     <col min="30" max="30" width="12.42578125" customWidth="1"/>
+    <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -913,31 +924,34 @@
       <c r="AD1" t="s">
         <v>15</v>
       </c>
+      <c r="AE1" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3">
-        <v>7582677255</v>
+        <v>78</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3861198309</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I2">
         <v>11111111</v>
@@ -949,16 +963,16 @@
         <v>40</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
         <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="P2" t="s">
         <v>41</v>
@@ -992,18 +1006,21 @@
         <v>STA017</v>
       </c>
       <c r="AB2" t="str">
-        <f>[1]Motor_Answer!$B2</f>
-        <v>ABC12STA017</v>
+        <f>[1]Motor_Answer!$B3</f>
+        <v>ABC12STA018</v>
       </c>
       <c r="AC2" t="str">
-        <f>[1]Motor_Answer!$C2</f>
-        <v>ZAZ123STA017</v>
+        <f>[1]Motor_Answer!$C3</f>
+        <v>ZAZ123STA018</v>
       </c>
       <c r="AD2" t="s">
         <v>19</v>
       </c>
+      <c r="AE2">
+        <v>32145234</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1027,12 +1044,6 @@
       </c>
       <c r="K3" t="s">
         <v>40</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
       </c>
       <c r="O3" t="s">
         <v>56</v>
@@ -1062,19 +1073,8 @@
         <f>[1]Motor_Answer!$A3</f>
         <v>STA018</v>
       </c>
-      <c r="AB3" t="str">
-        <f>[1]Motor_Answer!$B3</f>
-        <v>ABC12STA018</v>
-      </c>
-      <c r="AC3" t="str">
-        <f>[1]Motor_Answer!$C3</f>
-        <v>ZAZ123STA018</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1154,8 +1154,11 @@
       <c r="AD4" t="s">
         <v>19</v>
       </c>
+      <c r="AF4">
+        <v>23746788</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1454,7 +1457,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="Q12" s="10"/>
       <c r="R12" s="11"/>
       <c r="T12" s="9"/>
@@ -1698,7 +1701,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{C060C9A3-E5A4-403F-A29B-A6A88A5FC43D}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FA0BA8B5-8B3D-4994-A6EE-5B3C377C935F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>